<commit_message>
long time no comit
</commit_message>
<xml_diff>
--- a/product_data/processing_metadata/C1/PROF_meta.xlsx
+++ b/product_data/processing_metadata/C1/PROF_meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE/product_data/processing_metadata/C1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{D7290B6D-A588-472E-A3B0-67391D39AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A502831-0777-492D-A5B1-607F844DC22D}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{D7290B6D-A588-472E-A3B0-67391D39AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{584F7EBD-AD8B-4F0F-9B07-0D502DC59B5F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00480421-414C-413B-BC4D-00F98120957B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00480421-414C-413B-BC4D-00F98120957B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA997538-EC9F-42CD-BFDA-0538E4F1CABF}">
   <dimension ref="A1:BB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="A20:E20"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1807,7 +1807,7 @@
       <c r="AP7" t="s">
         <v>118</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AV7" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       <c r="AP12" t="s">
         <v>118</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AV12" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
       <c r="AP13" t="s">
         <v>118</v>
       </c>
-      <c r="AR13" t="s">
+      <c r="AV13" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>